<commit_message>
cool desc/stats tabs ...
</commit_message>
<xml_diff>
--- a/tabs/desc.xlsx
+++ b/tabs/desc.xlsx
@@ -10,8 +10,9 @@
     <sheet name="mean" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="sd" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="median" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="min" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="max" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="IQR" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="min" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="max" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -3900,22 +3901,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="G2" t="n">
-        <v>55</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -3923,22 +3924,22 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>4.75</v>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
+        <v>4.75</v>
       </c>
       <c r="D3" t="n">
-        <v>11</v>
+        <v>4.75</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G3" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -3946,22 +3947,22 @@
         <v>11</v>
       </c>
       <c r="B4" t="n">
-        <v>20</v>
+        <v>11.5</v>
       </c>
       <c r="C4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="G4" t="n">
         <v>21</v>
-      </c>
-      <c r="D4" t="n">
-        <v>22</v>
-      </c>
-      <c r="E4" t="n">
-        <v>23</v>
-      </c>
-      <c r="F4" t="n">
-        <v>29</v>
-      </c>
-      <c r="G4" t="n">
-        <v>23</v>
       </c>
     </row>
     <row r="5">
@@ -3969,22 +3970,22 @@
         <v>17</v>
       </c>
       <c r="B5" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D5" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
-        <v>29</v>
+        <v>11.5</v>
       </c>
       <c r="F5" t="n">
-        <v>30</v>
+        <v>7.5</v>
       </c>
       <c r="G5" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -3992,22 +3993,22 @@
         <v>18</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>9.25</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G6" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -4015,22 +4016,22 @@
         <v>19</v>
       </c>
       <c r="B7" t="n">
-        <v>126</v>
+        <v>4.75</v>
       </c>
       <c r="C7" t="n">
-        <v>131</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>126</v>
+        <v>4.25</v>
       </c>
       <c r="E7" t="n">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="G7" t="n">
-        <v>138</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -4038,22 +4039,22 @@
         <v>21</v>
       </c>
       <c r="B8" t="n">
-        <v>17</v>
+        <v>11.25</v>
       </c>
       <c r="C8" t="n">
-        <v>26</v>
+        <v>10.25</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>14.75</v>
       </c>
       <c r="E8" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="F8" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="9">
@@ -4061,22 +4062,22 @@
         <v>23</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -4084,22 +4085,22 @@
         <v>24</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>3.25</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="11">
@@ -4107,22 +4108,22 @@
         <v>25</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="12">
@@ -4130,22 +4131,22 @@
         <v>26</v>
       </c>
       <c r="B12" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E12" t="n">
         <v>3</v>
       </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>6</v>
-      </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="13">
@@ -4153,22 +4154,22 @@
         <v>27</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -4176,22 +4177,22 @@
         <v>28</v>
       </c>
       <c r="B14" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>6</v>
+        <v>8.5</v>
       </c>
       <c r="D14" t="n">
-        <v>17</v>
+        <v>8.5</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>9.25</v>
       </c>
       <c r="F14" t="n">
         <v>7</v>
       </c>
       <c r="G14" t="n">
-        <v>11</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="15">
@@ -4199,22 +4200,22 @@
         <v>29</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="D15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E15" t="n">
         <v>5</v>
       </c>
-      <c r="E15" t="n">
-        <v>1</v>
-      </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>3.75</v>
       </c>
       <c r="G15" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="16">
@@ -4222,22 +4223,22 @@
         <v>30</v>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17">
@@ -4268,22 +4269,22 @@
         <v>32</v>
       </c>
       <c r="B18" t="n">
-        <v>11.09</v>
+        <v>5.25</v>
       </c>
       <c r="C18" t="n">
-        <v>10.71</v>
+        <v>3.4725</v>
       </c>
       <c r="D18" t="n">
-        <v>10.52</v>
+        <v>6.8075</v>
       </c>
       <c r="E18" t="n">
-        <v>10.97</v>
+        <v>2.77</v>
       </c>
       <c r="F18" t="n">
-        <v>11.3</v>
+        <v>4.52</v>
       </c>
       <c r="G18" t="n">
-        <v>13.73</v>
+        <v>11.7275</v>
       </c>
     </row>
     <row r="19">
@@ -4291,22 +4292,22 @@
         <v>33</v>
       </c>
       <c r="B19" t="n">
-        <v>13.1</v>
+        <v>5.775</v>
       </c>
       <c r="C19" t="n">
-        <v>13.5</v>
+        <v>5.6775</v>
       </c>
       <c r="D19" t="n">
-        <v>12.56</v>
+        <v>5.2225</v>
       </c>
       <c r="E19" t="n">
-        <v>11.53</v>
+        <v>4.285</v>
       </c>
       <c r="F19" t="n">
-        <v>12.23</v>
+        <v>6.38</v>
       </c>
       <c r="G19" t="n">
-        <v>16.57</v>
+        <v>11.16</v>
       </c>
     </row>
     <row r="20">
@@ -4314,22 +4315,22 @@
         <v>34</v>
       </c>
       <c r="B20" t="n">
-        <v>20.52</v>
+        <v>11.915</v>
       </c>
       <c r="C20" t="n">
-        <v>19.4</v>
+        <v>13.3625</v>
       </c>
       <c r="D20" t="n">
-        <v>21.62</v>
+        <v>11.5025</v>
       </c>
       <c r="E20" t="n">
-        <v>23.75</v>
+        <v>13.575</v>
       </c>
       <c r="F20" t="n">
-        <v>18.48</v>
+        <v>15.595</v>
       </c>
       <c r="G20" t="n">
-        <v>22.48</v>
+        <v>16.165</v>
       </c>
     </row>
     <row r="21">
@@ -4337,19 +4338,19 @@
         <v>35</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -4360,22 +4361,22 @@
         <v>36</v>
       </c>
       <c r="B22" t="n">
-        <v>14</v>
+        <v>8.75</v>
       </c>
       <c r="C22" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D22" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>11</v>
+        <v>8.75</v>
       </c>
       <c r="F22" t="n">
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="23">
@@ -4383,22 +4384,22 @@
         <v>37</v>
       </c>
       <c r="B23" t="n">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="C23" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="E23" t="n">
         <v>3</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="n">
-        <v>2</v>
       </c>
       <c r="F23" t="n">
         <v>2</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="24">
@@ -4406,22 +4407,22 @@
         <v>38</v>
       </c>
       <c r="B24" t="n">
-        <v>24.21</v>
+        <v>20.6825</v>
       </c>
       <c r="C24" t="n">
-        <v>23.04</v>
+        <v>28.1275</v>
       </c>
       <c r="D24" t="n">
-        <v>27.1</v>
+        <v>14.705</v>
       </c>
       <c r="E24" t="n">
-        <v>17.18</v>
+        <v>30.63</v>
       </c>
       <c r="F24" t="n">
-        <v>28.23</v>
+        <v>24.8225</v>
       </c>
       <c r="G24" t="n">
-        <v>32.7</v>
+        <v>51.7225</v>
       </c>
     </row>
     <row r="25">
@@ -4429,22 +4430,22 @@
         <v>39</v>
       </c>
       <c r="B25" t="n">
-        <v>37.72</v>
+        <v>78.82</v>
       </c>
       <c r="C25" t="n">
-        <v>47.69</v>
+        <v>102.91</v>
       </c>
       <c r="D25" t="n">
-        <v>58.91</v>
+        <v>66.5925</v>
       </c>
       <c r="E25" t="n">
-        <v>57.59</v>
+        <v>79.4</v>
       </c>
       <c r="F25" t="n">
-        <v>58.85</v>
+        <v>81.8</v>
       </c>
       <c r="G25" t="n">
-        <v>76</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26">
@@ -4452,22 +4453,22 @@
         <v>40</v>
       </c>
       <c r="B26" t="n">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="C26" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="D26" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="E26" t="n">
         <v>7</v>
       </c>
-      <c r="D26" t="n">
-        <v>12</v>
-      </c>
-      <c r="E26" t="n">
-        <v>3</v>
-      </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>6.25</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="27">
@@ -4475,22 +4476,22 @@
         <v>41</v>
       </c>
       <c r="B27" t="n">
-        <v>16</v>
+        <v>2.75</v>
       </c>
       <c r="C27" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D27" t="n">
-        <v>20</v>
+        <v>3.75</v>
       </c>
       <c r="E27" t="n">
-        <v>10</v>
+        <v>6.5</v>
       </c>
       <c r="F27" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G27" t="n">
-        <v>19</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="28">
@@ -4498,22 +4499,22 @@
         <v>42</v>
       </c>
       <c r="B28" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C28" t="n">
-        <v>11</v>
+        <v>0.75</v>
       </c>
       <c r="D28" t="n">
-        <v>12</v>
+        <v>2.25</v>
       </c>
       <c r="E28" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G28" t="n">
-        <v>14</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="29">
@@ -4521,22 +4522,22 @@
         <v>43</v>
       </c>
       <c r="B29" t="n">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="C29" t="n">
-        <v>9</v>
+        <v>6.75</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>8.75</v>
       </c>
       <c r="F29" t="n">
-        <v>6</v>
+        <v>10.25</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="30">
@@ -4544,22 +4545,22 @@
         <v>44</v>
       </c>
       <c r="B30" t="n">
-        <v>5</v>
+        <v>5.75</v>
       </c>
       <c r="C30" t="n">
-        <v>9</v>
+        <v>4.75</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>8.25</v>
       </c>
       <c r="F30" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
@@ -4567,22 +4568,22 @@
         <v>45</v>
       </c>
       <c r="B31" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C31" t="n">
-        <v>6</v>
+        <v>4.75</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="E31" t="n">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="F31" t="n">
-        <v>4</v>
+        <v>9.25</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="32">
@@ -4590,22 +4591,22 @@
         <v>46</v>
       </c>
       <c r="B32" t="n">
-        <v>9</v>
+        <v>11.5</v>
       </c>
       <c r="C32" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E32" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F32" t="n">
-        <v>9</v>
+        <v>10.75</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
@@ -4613,22 +4614,22 @@
         <v>47</v>
       </c>
       <c r="B33" t="n">
-        <v>4</v>
+        <v>5.75</v>
       </c>
       <c r="C33" t="n">
         <v>4</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>9.25</v>
       </c>
       <c r="E33" t="n">
+        <v>3</v>
+      </c>
+      <c r="F33" t="n">
         <v>6</v>
       </c>
-      <c r="F33" t="n">
-        <v>7</v>
-      </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="34">
@@ -4636,22 +4637,22 @@
         <v>48</v>
       </c>
       <c r="B34" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C34" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D34" t="n">
-        <v>26</v>
+        <v>2.25</v>
       </c>
       <c r="E34" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="G34" t="n">
-        <v>25</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="35">
@@ -4659,22 +4660,22 @@
         <v>49</v>
       </c>
       <c r="B35" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C35" t="n">
-        <v>27</v>
+        <v>1.75</v>
       </c>
       <c r="D35" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="F35" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -4682,22 +4683,22 @@
         <v>51</v>
       </c>
       <c r="B36" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="F36" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4742,6 +4743,848 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
+        <v>52</v>
+      </c>
+      <c r="C2" t="n">
+        <v>52</v>
+      </c>
+      <c r="D2" t="n">
+        <v>52</v>
+      </c>
+      <c r="E2" t="n">
+        <v>55</v>
+      </c>
+      <c r="F2" t="n">
+        <v>55</v>
+      </c>
+      <c r="G2" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11</v>
+      </c>
+      <c r="D3" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3" t="n">
+        <v>11</v>
+      </c>
+      <c r="F3" t="n">
+        <v>11</v>
+      </c>
+      <c r="G3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n">
+        <v>21</v>
+      </c>
+      <c r="D4" t="n">
+        <v>22</v>
+      </c>
+      <c r="E4" t="n">
+        <v>23</v>
+      </c>
+      <c r="F4" t="n">
+        <v>29</v>
+      </c>
+      <c r="G4" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="n">
+        <v>21</v>
+      </c>
+      <c r="C5" t="n">
+        <v>21</v>
+      </c>
+      <c r="D5" t="n">
+        <v>30</v>
+      </c>
+      <c r="E5" t="n">
+        <v>29</v>
+      </c>
+      <c r="F5" t="n">
+        <v>30</v>
+      </c>
+      <c r="G5" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="n">
+        <v>126</v>
+      </c>
+      <c r="C7" t="n">
+        <v>131</v>
+      </c>
+      <c r="D7" t="n">
+        <v>126</v>
+      </c>
+      <c r="E7" t="n">
+        <v>124</v>
+      </c>
+      <c r="F7" t="n">
+        <v>126</v>
+      </c>
+      <c r="G7" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="n">
+        <v>17</v>
+      </c>
+      <c r="C8" t="n">
+        <v>26</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>27</v>
+      </c>
+      <c r="F8" t="n">
+        <v>25</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>6</v>
+      </c>
+      <c r="D14" t="n">
+        <v>17</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="n">
+        <v>7</v>
+      </c>
+      <c r="G14" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="n">
+        <v>11.09</v>
+      </c>
+      <c r="C18" t="n">
+        <v>10.71</v>
+      </c>
+      <c r="D18" t="n">
+        <v>10.52</v>
+      </c>
+      <c r="E18" t="n">
+        <v>10.97</v>
+      </c>
+      <c r="F18" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="G18" t="n">
+        <v>13.73</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="n">
+        <v>13.1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="D19" t="n">
+        <v>12.56</v>
+      </c>
+      <c r="E19" t="n">
+        <v>11.53</v>
+      </c>
+      <c r="F19" t="n">
+        <v>12.23</v>
+      </c>
+      <c r="G19" t="n">
+        <v>16.57</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20.52</v>
+      </c>
+      <c r="C20" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="D20" t="n">
+        <v>21.62</v>
+      </c>
+      <c r="E20" t="n">
+        <v>23.75</v>
+      </c>
+      <c r="F20" t="n">
+        <v>18.48</v>
+      </c>
+      <c r="G20" t="n">
+        <v>22.48</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="n">
+        <v>14</v>
+      </c>
+      <c r="C22" t="n">
+        <v>13</v>
+      </c>
+      <c r="D22" t="n">
+        <v>12</v>
+      </c>
+      <c r="E22" t="n">
+        <v>11</v>
+      </c>
+      <c r="F22" t="n">
+        <v>12</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="n">
+        <v>5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>3</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="n">
+        <v>24.21</v>
+      </c>
+      <c r="C24" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="D24" t="n">
+        <v>27.1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>17.18</v>
+      </c>
+      <c r="F24" t="n">
+        <v>28.23</v>
+      </c>
+      <c r="G24" t="n">
+        <v>32.7</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="n">
+        <v>37.72</v>
+      </c>
+      <c r="C25" t="n">
+        <v>47.69</v>
+      </c>
+      <c r="D25" t="n">
+        <v>58.91</v>
+      </c>
+      <c r="E25" t="n">
+        <v>57.59</v>
+      </c>
+      <c r="F25" t="n">
+        <v>58.85</v>
+      </c>
+      <c r="G25" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" t="n">
+        <v>7</v>
+      </c>
+      <c r="D26" t="n">
+        <v>12</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="n">
+        <v>16</v>
+      </c>
+      <c r="C27" t="n">
+        <v>19</v>
+      </c>
+      <c r="D27" t="n">
+        <v>20</v>
+      </c>
+      <c r="E27" t="n">
+        <v>10</v>
+      </c>
+      <c r="F27" t="n">
+        <v>15</v>
+      </c>
+      <c r="G27" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="n">
+        <v>12</v>
+      </c>
+      <c r="C28" t="n">
+        <v>11</v>
+      </c>
+      <c r="D28" t="n">
+        <v>12</v>
+      </c>
+      <c r="E28" t="n">
+        <v>8</v>
+      </c>
+      <c r="F28" t="n">
+        <v>12</v>
+      </c>
+      <c r="G28" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" t="n">
+        <v>7</v>
+      </c>
+      <c r="C29" t="n">
+        <v>9</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>6</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" t="n">
+        <v>5</v>
+      </c>
+      <c r="C30" t="n">
+        <v>9</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>4</v>
+      </c>
+      <c r="F30" t="n">
+        <v>3</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="n">
+        <v>8</v>
+      </c>
+      <c r="C31" t="n">
+        <v>6</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>4</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="n">
+        <v>9</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>11</v>
+      </c>
+      <c r="F32" t="n">
+        <v>9</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" t="n">
+        <v>4</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>6</v>
+      </c>
+      <c r="F33" t="n">
+        <v>7</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="n">
+        <v>20</v>
+      </c>
+      <c r="C34" t="n">
+        <v>22</v>
+      </c>
+      <c r="D34" t="n">
+        <v>26</v>
+      </c>
+      <c r="E34" t="n">
+        <v>21</v>
+      </c>
+      <c r="F34" t="n">
+        <v>25</v>
+      </c>
+      <c r="G34" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" t="n">
+        <v>25</v>
+      </c>
+      <c r="C35" t="n">
+        <v>27</v>
+      </c>
+      <c r="D35" t="n">
+        <v>28</v>
+      </c>
+      <c r="E35" t="n">
+        <v>23</v>
+      </c>
+      <c r="F35" t="n">
+        <v>25</v>
+      </c>
+      <c r="G35" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="n">
+        <v>26</v>
+      </c>
+      <c r="C36" t="n">
+        <v>29</v>
+      </c>
+      <c r="D36" t="n">
+        <v>30</v>
+      </c>
+      <c r="E36" t="n">
+        <v>27</v>
+      </c>
+      <c r="F36" t="n">
+        <v>28</v>
+      </c>
+      <c r="G36" t="n">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="n">
         <v>82</v>
       </c>
       <c r="C2" t="n">

</xml_diff>